<commit_message>
240930, literacy modified 2
</commit_message>
<xml_diff>
--- a/R/data/quiz241007.xlsx
+++ b/R/data/quiz241007.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Dropbox/내 Mac (Kee-Won의 MacBook Air)/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFBE927-6158-D040-9468-B81AC06D00EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46237789-B4D9-1641-B0FC-9D19A7F4832E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8560" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2780" yWindow="2660" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설문지 응답 시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3744" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4063" uniqueCount="931">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2610,6 +2610,210 @@
   </si>
   <si>
     <t>김나현</t>
+  </si>
+  <si>
+    <t>cgb01045647472@gmail.com</t>
+  </si>
+  <si>
+    <t>최기백</t>
+  </si>
+  <si>
+    <t>wnsrl2498@naver.com</t>
+  </si>
+  <si>
+    <t>김준기</t>
+  </si>
+  <si>
+    <t>ystop061012@naver.com</t>
+  </si>
+  <si>
+    <t>손연수</t>
+  </si>
+  <si>
+    <t>orienfun@gmail.com</t>
+  </si>
+  <si>
+    <t>이동화</t>
+  </si>
+  <si>
+    <t>dearmy0819@gmail.com</t>
+  </si>
+  <si>
+    <t>박혜원</t>
+  </si>
+  <si>
+    <t>kesha11@naver.com</t>
+  </si>
+  <si>
+    <t>윤주호</t>
+  </si>
+  <si>
+    <t>shasha4321@naver.com</t>
+  </si>
+  <si>
+    <t>정다영</t>
+  </si>
+  <si>
+    <t>qkhkasin17@naver.com</t>
+  </si>
+  <si>
+    <t>박가현</t>
+  </si>
+  <si>
+    <t>to_csm@naver.com</t>
+  </si>
+  <si>
+    <t>천상미</t>
+  </si>
+  <si>
+    <t>harypoter8947@gmail.com</t>
+  </si>
+  <si>
+    <t>김석희</t>
+  </si>
+  <si>
+    <t>ncu11069@naver.com</t>
+  </si>
+  <si>
+    <t>이규민</t>
+  </si>
+  <si>
+    <t>dlakrp731@gmail.com</t>
+  </si>
+  <si>
+    <t>콘텐츠it</t>
+  </si>
+  <si>
+    <t>이준수</t>
+  </si>
+  <si>
+    <t>leyy2k@naver.com</t>
+  </si>
+  <si>
+    <t>김대현</t>
+  </si>
+  <si>
+    <t>dbfrhr02@naver.com</t>
+  </si>
+  <si>
+    <t>심건휘</t>
+  </si>
+  <si>
+    <t>jiminn101777@gmail.com</t>
+  </si>
+  <si>
+    <t>권지민</t>
+  </si>
+  <si>
+    <t>csm06125@naver.com</t>
+  </si>
+  <si>
+    <t>박근태</t>
+  </si>
+  <si>
+    <t>qortjdus27@naver.com</t>
+  </si>
+  <si>
+    <t>백서연</t>
+  </si>
+  <si>
+    <t>coreykang3@naver.com</t>
+  </si>
+  <si>
+    <t>반도체공학</t>
+  </si>
+  <si>
+    <t>강동훈</t>
+  </si>
+  <si>
+    <t>kimguswls6685@naver.com</t>
+  </si>
+  <si>
+    <t>김현진</t>
+  </si>
+  <si>
+    <t>jiah1622@naver.com</t>
+  </si>
+  <si>
+    <t>최지아</t>
+  </si>
+  <si>
+    <t>seungye04@naver.com</t>
+  </si>
+  <si>
+    <t>언론방송융합미디어</t>
+  </si>
+  <si>
+    <t>정승예</t>
+  </si>
+  <si>
+    <t>lucy37lucy37lucy37@naver.com</t>
+  </si>
+  <si>
+    <t>이은지</t>
+  </si>
+  <si>
+    <t>dustinwon2005@gmail.com</t>
+  </si>
+  <si>
+    <t>원지현</t>
+  </si>
+  <si>
+    <t>minuhwang16@gmail.com</t>
+  </si>
+  <si>
+    <t>황민우</t>
+  </si>
+  <si>
+    <t>chsmdfur123@naver.com</t>
+  </si>
+  <si>
+    <t>금융재무</t>
+  </si>
+  <si>
+    <t>이한얼</t>
+  </si>
+  <si>
+    <t>jwtp724@naver.com</t>
+  </si>
+  <si>
+    <t>박이선</t>
+  </si>
+  <si>
+    <t>lyn392392@naver.com</t>
+  </si>
+  <si>
+    <t>이유나</t>
+  </si>
+  <si>
+    <t>happyrovot88@gmail.com</t>
+  </si>
+  <si>
+    <t>김도연</t>
+  </si>
+  <si>
+    <t>eunsoljj12@gmail.com</t>
+  </si>
+  <si>
+    <t>권은솔</t>
+  </si>
+  <si>
+    <t>juhui050356@naver.com</t>
+  </si>
+  <si>
+    <t>김주희</t>
+  </si>
+  <si>
+    <t>5tmddk@naver.com</t>
+  </si>
+  <si>
+    <t>최승아</t>
+  </si>
+  <si>
+    <t>chhs337@naver.com</t>
+  </si>
+  <si>
+    <t>최홍서</t>
   </si>
 </sst>
 </file>
@@ -3025,7 +3229,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N374" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N406" headerRowCount="0">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -3252,11 +3456,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N374"/>
+  <dimension ref="A1:N406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A351" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B380" sqref="B380"/>
+      <pane ySplit="1" topLeftCell="A388" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18682,8 +18886,1320 @@
       <c r="L374" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M374" s="26"/>
       <c r="N374" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="375" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A375" s="8">
+        <v>45578.619641469908</v>
+      </c>
+      <c r="B375" s="9" t="s">
+        <v>863</v>
+      </c>
+      <c r="C375" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D375" s="9">
+        <v>20193003</v>
+      </c>
+      <c r="E375" s="9" t="s">
+        <v>864</v>
+      </c>
+      <c r="F375" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G375" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H375" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I375" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J375" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K375" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L375" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N375" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="376" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A376" s="4">
+        <v>45578.640179502312</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="C376" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D376" s="5">
+        <v>20227093</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="F376" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G376" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H376" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I376" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J376" s="6">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K376" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L376" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M376" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="377" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A377" s="8">
+        <v>45578.656618159723</v>
+      </c>
+      <c r="B377" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="C377" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D377" s="9">
+        <v>20246628</v>
+      </c>
+      <c r="E377" s="9" t="s">
+        <v>868</v>
+      </c>
+      <c r="F377" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G377" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="H377" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I377" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J377" s="10">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K377" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L377" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N377" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="378" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A378" s="4">
+        <v>45578.662793564814</v>
+      </c>
+      <c r="B378" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="C378" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D378" s="5">
+        <v>20245218</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="F378" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G378" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H378" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I378" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J378" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K378" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L378" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M378" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="379" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A379" s="8">
+        <v>45578.66937581019</v>
+      </c>
+      <c r="B379" s="9" t="s">
+        <v>871</v>
+      </c>
+      <c r="C379" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D379" s="9">
+        <v>20243225</v>
+      </c>
+      <c r="E379" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="F379" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G379" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H379" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I379" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J379" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K379" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L379" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N379" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="380" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A380" s="4">
+        <v>45578.674752708335</v>
+      </c>
+      <c r="B380" s="5" t="s">
+        <v>873</v>
+      </c>
+      <c r="C380" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D380" s="5">
+        <v>20211059</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="F380" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H380" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I380" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J380" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K380" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L380" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N380" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="381" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A381" s="8">
+        <v>45578.675853402776</v>
+      </c>
+      <c r="B381" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="C381" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="D381" s="9">
+        <v>20213035</v>
+      </c>
+      <c r="E381" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="F381" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G381" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H381" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I381" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J381" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K381" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L381" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N381" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="382" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A382" s="4">
+        <v>45578.677845995371</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D382" s="5">
+        <v>20232953</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="F382" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H382" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I382" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J382" s="12">
+        <v>0.72</v>
+      </c>
+      <c r="K382" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L382" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M382" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="383" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A383" s="8">
+        <v>45578.699198993054</v>
+      </c>
+      <c r="B383" s="9" t="s">
+        <v>879</v>
+      </c>
+      <c r="C383" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D383" s="9">
+        <v>20242844</v>
+      </c>
+      <c r="E383" s="9" t="s">
+        <v>880</v>
+      </c>
+      <c r="F383" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G383" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H383" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I383" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J383" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K383" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L383" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N383" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="384" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A384" s="4">
+        <v>45578.704304120372</v>
+      </c>
+      <c r="B384" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="C384" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D384" s="5">
+        <v>20231205</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="F384" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G384" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H384" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I384" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J384" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K384" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L384" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N384" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="385" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A385" s="8">
+        <v>45578.70438841435</v>
+      </c>
+      <c r="B385" s="9" t="s">
+        <v>883</v>
+      </c>
+      <c r="C385" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D385" s="9">
+        <v>20231622</v>
+      </c>
+      <c r="E385" s="9" t="s">
+        <v>884</v>
+      </c>
+      <c r="F385" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G385" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H385" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I385" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J385" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K385" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L385" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M385" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="386" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A386" s="4">
+        <v>45578.704891921298</v>
+      </c>
+      <c r="B386" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="C386" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="D386" s="5">
+        <v>20195225</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="F386" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G386" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H386" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I386" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J386" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K386" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L386" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M386" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="387" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A387" s="8">
+        <v>45578.710554791665</v>
+      </c>
+      <c r="B387" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="C387" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="D387" s="9">
+        <v>20215115</v>
+      </c>
+      <c r="E387" s="9" t="s">
+        <v>889</v>
+      </c>
+      <c r="F387" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G387" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H387" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I387" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J387" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K387" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L387" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M387" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="388" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A388" s="4">
+        <v>45578.72470421296</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="C388" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D388" s="5">
+        <v>20212971</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="F388" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G388" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H388" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I388" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J388" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K388" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L388" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M388" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="389" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A389" s="8">
+        <v>45578.729495300926</v>
+      </c>
+      <c r="B389" s="9" t="s">
+        <v>892</v>
+      </c>
+      <c r="C389" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D389" s="9">
+        <v>20242306</v>
+      </c>
+      <c r="E389" s="9" t="s">
+        <v>893</v>
+      </c>
+      <c r="F389" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G389" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H389" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I389" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J389" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K389" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L389" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N389" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="390" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A390" s="4">
+        <v>45578.737708738423</v>
+      </c>
+      <c r="B390" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D390" s="5">
+        <v>20203321</v>
+      </c>
+      <c r="E390" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="F390" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G390" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H390" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I390" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J390" s="6">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="K390" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L390" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N390" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="391" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A391" s="8">
+        <v>45578.740375532405</v>
+      </c>
+      <c r="B391" s="9" t="s">
+        <v>896</v>
+      </c>
+      <c r="C391" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D391" s="9">
+        <v>20242971</v>
+      </c>
+      <c r="E391" s="9" t="s">
+        <v>897</v>
+      </c>
+      <c r="F391" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G391" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H391" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I391" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J391" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K391" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L391" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M391" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="392" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A392" s="4">
+        <v>45578.744304305554</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="D392" s="5">
+        <v>20233301</v>
+      </c>
+      <c r="E392" s="5" t="s">
+        <v>900</v>
+      </c>
+      <c r="F392" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H392" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I392" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J392" s="6">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K392" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L392" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N392" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="393" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A393" s="8">
+        <v>45578.744441585644</v>
+      </c>
+      <c r="B393" s="9" t="s">
+        <v>901</v>
+      </c>
+      <c r="C393" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D393" s="9">
+        <v>20215144</v>
+      </c>
+      <c r="E393" s="9" t="s">
+        <v>902</v>
+      </c>
+      <c r="F393" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G393" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H393" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I393" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J393" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K393" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L393" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M393" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="394" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A394" s="4">
+        <v>45578.764729849536</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D394" s="5">
+        <v>20245271</v>
+      </c>
+      <c r="E394" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="F394" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G394" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H394" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I394" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J394" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K394" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L394" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N394" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="395" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A395" s="8">
+        <v>45578.77320747685</v>
+      </c>
+      <c r="B395" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="C395" s="9" t="s">
+        <v>906</v>
+      </c>
+      <c r="D395" s="9">
+        <v>20233846</v>
+      </c>
+      <c r="E395" s="9" t="s">
+        <v>907</v>
+      </c>
+      <c r="F395" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G395" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H395" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I395" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J395" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K395" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L395" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N395" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="396" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A396" s="4">
+        <v>45578.775014016202</v>
+      </c>
+      <c r="B396" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="C396" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D396" s="5">
+        <v>20223010</v>
+      </c>
+      <c r="E396" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="F396" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G396" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H396" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I396" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J396" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K396" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L396" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N396" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="397" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A397" s="8">
+        <v>45578.781653692131</v>
+      </c>
+      <c r="B397" s="9" t="s">
+        <v>910</v>
+      </c>
+      <c r="C397" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D397" s="9">
+        <v>20246747</v>
+      </c>
+      <c r="E397" s="9" t="s">
+        <v>911</v>
+      </c>
+      <c r="F397" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G397" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H397" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I397" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J397" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="K397" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L397" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N397" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="398" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A398" s="4">
+        <v>45578.781885682867</v>
+      </c>
+      <c r="B398" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="C398" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D398" s="5">
+        <v>20243967</v>
+      </c>
+      <c r="E398" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="F398" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G398" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H398" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I398" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J398" s="6">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K398" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="L398" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M398" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="399" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A399" s="8">
+        <v>45578.789774050922</v>
+      </c>
+      <c r="B399" s="9" t="s">
+        <v>914</v>
+      </c>
+      <c r="C399" s="9" t="s">
+        <v>915</v>
+      </c>
+      <c r="D399" s="9">
+        <v>20203026</v>
+      </c>
+      <c r="E399" s="9" t="s">
+        <v>916</v>
+      </c>
+      <c r="F399" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G399" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H399" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I399" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J399" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K399" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L399" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N399" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="400" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A400" s="4">
+        <v>45578.793432013888</v>
+      </c>
+      <c r="B400" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="C400" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D400" s="5">
+        <v>20206504</v>
+      </c>
+      <c r="E400" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="F400" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G400" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H400" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I400" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J400" s="6">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K400" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L400" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N400" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="401" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A401" s="8">
+        <v>45578.798768333334</v>
+      </c>
+      <c r="B401" s="9" t="s">
+        <v>919</v>
+      </c>
+      <c r="C401" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D401" s="9">
+        <v>20243007</v>
+      </c>
+      <c r="E401" s="9" t="s">
+        <v>920</v>
+      </c>
+      <c r="F401" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G401" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H401" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I401" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J401" s="10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K401" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L401" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M401" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="402" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A402" s="4">
+        <v>45578.813740995371</v>
+      </c>
+      <c r="B402" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="C402" s="5">
+        <v>20242919</v>
+      </c>
+      <c r="D402" s="5">
+        <v>20242919</v>
+      </c>
+      <c r="E402" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="F402" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G402" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H402" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I402" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J402" s="6">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K402" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L402" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M402" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="403" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A403" s="8">
+        <v>45578.820547048614</v>
+      </c>
+      <c r="B403" s="9" t="s">
+        <v>923</v>
+      </c>
+      <c r="C403" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="D403" s="9">
+        <v>20245113</v>
+      </c>
+      <c r="E403" s="9" t="s">
+        <v>924</v>
+      </c>
+      <c r="F403" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G403" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H403" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I403" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J403" s="16">
+        <v>0.72</v>
+      </c>
+      <c r="K403" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L403" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N403" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="404" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A404" s="4">
+        <v>45578.822771724532</v>
+      </c>
+      <c r="B404" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="C404" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D404" s="5">
+        <v>20242111</v>
+      </c>
+      <c r="E404" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="F404" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G404" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H404" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I404" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J404" s="12">
+        <v>0.72</v>
+      </c>
+      <c r="K404" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L404" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M404" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="405" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A405" s="8">
+        <v>45578.825338796298</v>
+      </c>
+      <c r="B405" s="9" t="s">
+        <v>927</v>
+      </c>
+      <c r="C405" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D405" s="9">
+        <v>20192634</v>
+      </c>
+      <c r="E405" s="9" t="s">
+        <v>928</v>
+      </c>
+      <c r="F405" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G405" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H405" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I405" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J405" s="10">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="K405" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L405" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M405" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="406" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A406" s="17">
+        <v>45578.833702152777</v>
+      </c>
+      <c r="B406" s="18" t="s">
+        <v>929</v>
+      </c>
+      <c r="C406" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D406" s="18">
+        <v>20183006</v>
+      </c>
+      <c r="E406" s="18" t="s">
+        <v>930</v>
+      </c>
+      <c r="F406" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G406" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H406" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I406" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J406" s="19">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K406" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="L406" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M406" s="26"/>
+      <c r="N406" s="20" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>